<commit_message>
Ajustes para manipular calculadora
</commit_message>
<xml_diff>
--- a/arquivo_excel.xlsx
+++ b/arquivo_excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Nome do fornecedor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor Total</t>
   </si>
   <si>
     <t xml:space="preserve">Data de vencimento</t>
@@ -174,7 +171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,10 +222,6 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -311,7 +304,7 @@
   <dimension ref="A1:AMJ132"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -319,8 +312,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="4" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -351,10 +344,8 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
@@ -368,30 +359,27 @@
         <v>45169</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>20000</v>
-      </c>
-      <c r="E2" s="5" t="n">
+      <c r="D2" s="5" t="n">
         <v>45171</v>
       </c>
+      <c r="E2" s="7" t="n">
+        <v>1500</v>
+      </c>
       <c r="F2" s="7" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G2" s="7" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="7" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="7" t="n">
-        <v>2000</v>
-      </c>
       <c r="I2" s="7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J2" s="7" t="n">
         <v>1500</v>
       </c>
     </row>
@@ -400,241 +388,218 @@
         <v>45199</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E3" s="8" t="n">
+      <c r="D3" s="8" t="n">
         <v>45201</v>
       </c>
+      <c r="E3" s="10" t="n">
+        <v>150</v>
+      </c>
       <c r="F3" s="10" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="G3" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="H3" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
-        <v>14</v>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="12"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="13"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C132" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>